<commit_message>
CIERRE 23 MAYO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="281">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1158,6 +1158,15 @@
   </si>
   <si>
     <t>BALANCE      ABASTO 4 CARNES    H E R R A D U R A    MAYO        2 0 2 2</t>
+  </si>
+  <si>
+    <t>NOMINA # 19</t>
+  </si>
+  <si>
+    <t>LONGANIZA-ARABE</t>
+  </si>
+  <si>
+    <t>NOMINA # 20</t>
   </si>
 </sst>
 </file>
@@ -2926,6 +2935,56 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="27" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3007,58 +3066,8 @@
     <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="27" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5508,23 +5517,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="292"/>
-      <c r="C1" s="294" t="s">
+      <c r="B1" s="274"/>
+      <c r="C1" s="276" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="293"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -5534,21 +5543,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="279"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="280"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="265" t="s">
+      <c r="R3" s="285" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5563,14 +5572,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="281" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="282"/>
+      <c r="H4" s="283" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="284"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -5580,11 +5589,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="272" t="s">
+      <c r="P4" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="273"/>
-      <c r="R4" s="266"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="286"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -7085,11 +7094,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="274">
+      <c r="M40" s="294">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="276">
+      <c r="N40" s="296">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -7115,8 +7124,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="275"/>
-      <c r="N41" s="277"/>
+      <c r="M41" s="295"/>
+      <c r="N41" s="297"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -7331,29 +7340,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="299"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="280">
+      <c r="K53" s="300">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="282">
+      <c r="L53" s="301"/>
+      <c r="M53" s="302">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="283"/>
+      <c r="N53" s="303"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="284" t="s">
+      <c r="D54" s="304" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="284"/>
+      <c r="E54" s="304"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -7364,22 +7373,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="285" t="s">
+      <c r="D55" s="305" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="285"/>
+      <c r="E55" s="305"/>
       <c r="F55" s="115">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="286" t="s">
+      <c r="I55" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="287"/>
-      <c r="K55" s="288">
+      <c r="J55" s="307"/>
+      <c r="K55" s="308">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="289"/>
+      <c r="L55" s="309"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -7410,11 +7419,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="290">
+      <c r="K57" s="310">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="291"/>
+      <c r="L57" s="311"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -7431,22 +7440,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="267" t="s">
+      <c r="D59" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="268"/>
+      <c r="E59" s="288"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="269" t="s">
+      <c r="I59" s="289" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="270"/>
-      <c r="K59" s="271">
+      <c r="J59" s="290"/>
+      <c r="K59" s="291">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="271"/>
+      <c r="L59" s="291"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -7590,12 +7599,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -7611,6 +7614,12 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7674,21 +7683,21 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="304"/>
-      <c r="B3" s="305"/>
-      <c r="C3" s="306"/>
-      <c r="D3" s="307"/>
-      <c r="E3" s="306"/>
+      <c r="A3" s="265"/>
+      <c r="B3" s="266"/>
+      <c r="C3" s="267"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="267"/>
       <c r="F3" s="158">
         <f>C3-E3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="308"/>
-      <c r="B4" s="309"/>
+      <c r="A4" s="269"/>
+      <c r="B4" s="270"/>
       <c r="C4" s="132"/>
-      <c r="D4" s="310"/>
+      <c r="D4" s="271"/>
       <c r="E4" s="132"/>
       <c r="F4" s="196">
         <f>C4-E4+F3</f>
@@ -7696,10 +7705,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="308"/>
-      <c r="B5" s="309"/>
+      <c r="A5" s="269"/>
+      <c r="B5" s="270"/>
       <c r="C5" s="132"/>
-      <c r="D5" s="310"/>
+      <c r="D5" s="271"/>
       <c r="E5" s="132"/>
       <c r="F5" s="196">
         <f t="shared" ref="F5:F68" si="0">C5-E5+F4</f>
@@ -7707,10 +7716,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="308"/>
-      <c r="B6" s="309"/>
+      <c r="A6" s="269"/>
+      <c r="B6" s="270"/>
       <c r="C6" s="132"/>
-      <c r="D6" s="310"/>
+      <c r="D6" s="271"/>
       <c r="E6" s="132"/>
       <c r="F6" s="196">
         <f t="shared" si="0"/>
@@ -7719,10 +7728,10 @@
       <c r="G6" s="162"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="308"/>
-      <c r="B7" s="309"/>
+      <c r="A7" s="269"/>
+      <c r="B7" s="270"/>
       <c r="C7" s="132"/>
-      <c r="D7" s="310"/>
+      <c r="D7" s="271"/>
       <c r="E7" s="132"/>
       <c r="F7" s="196">
         <f t="shared" si="0"/>
@@ -7730,10 +7739,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="308"/>
-      <c r="B8" s="309"/>
+      <c r="A8" s="269"/>
+      <c r="B8" s="270"/>
       <c r="C8" s="132"/>
-      <c r="D8" s="310"/>
+      <c r="D8" s="271"/>
       <c r="E8" s="132"/>
       <c r="F8" s="196">
         <f t="shared" si="0"/>
@@ -7741,10 +7750,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="308"/>
-      <c r="B9" s="309"/>
+      <c r="A9" s="269"/>
+      <c r="B9" s="270"/>
       <c r="C9" s="132"/>
-      <c r="D9" s="310"/>
+      <c r="D9" s="271"/>
       <c r="E9" s="132"/>
       <c r="F9" s="196">
         <f t="shared" si="0"/>
@@ -7752,10 +7761,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="308"/>
-      <c r="B10" s="309"/>
+      <c r="A10" s="269"/>
+      <c r="B10" s="270"/>
       <c r="C10" s="132"/>
-      <c r="D10" s="310"/>
+      <c r="D10" s="271"/>
       <c r="E10" s="132"/>
       <c r="F10" s="196">
         <f t="shared" si="0"/>
@@ -7763,10 +7772,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="308"/>
-      <c r="B11" s="309"/>
+      <c r="A11" s="269"/>
+      <c r="B11" s="270"/>
       <c r="C11" s="132"/>
-      <c r="D11" s="310"/>
+      <c r="D11" s="271"/>
       <c r="E11" s="132"/>
       <c r="F11" s="196">
         <f t="shared" si="0"/>
@@ -7774,10 +7783,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="308"/>
-      <c r="B12" s="309"/>
+      <c r="A12" s="269"/>
+      <c r="B12" s="270"/>
       <c r="C12" s="132"/>
-      <c r="D12" s="310"/>
+      <c r="D12" s="271"/>
       <c r="E12" s="132"/>
       <c r="F12" s="196">
         <f t="shared" si="0"/>
@@ -7786,10 +7795,10 @@
       <c r="G12" s="162"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="308"/>
-      <c r="B13" s="309"/>
+      <c r="A13" s="269"/>
+      <c r="B13" s="270"/>
       <c r="C13" s="132"/>
-      <c r="D13" s="310"/>
+      <c r="D13" s="271"/>
       <c r="E13" s="132"/>
       <c r="F13" s="196">
         <f t="shared" si="0"/>
@@ -7797,10 +7806,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="308"/>
-      <c r="B14" s="309"/>
+      <c r="A14" s="269"/>
+      <c r="B14" s="270"/>
       <c r="C14" s="132"/>
-      <c r="D14" s="310"/>
+      <c r="D14" s="271"/>
       <c r="E14" s="132"/>
       <c r="F14" s="196">
         <f t="shared" si="0"/>
@@ -7808,10 +7817,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="308"/>
-      <c r="B15" s="309"/>
+      <c r="A15" s="269"/>
+      <c r="B15" s="270"/>
       <c r="C15" s="132"/>
-      <c r="D15" s="310"/>
+      <c r="D15" s="271"/>
       <c r="E15" s="132"/>
       <c r="F15" s="196">
         <f t="shared" si="0"/>
@@ -7819,10 +7828,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="308"/>
-      <c r="B16" s="309"/>
+      <c r="A16" s="269"/>
+      <c r="B16" s="270"/>
       <c r="C16" s="132"/>
-      <c r="D16" s="310"/>
+      <c r="D16" s="271"/>
       <c r="E16" s="132"/>
       <c r="F16" s="196">
         <f t="shared" si="0"/>
@@ -7830,10 +7839,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="308"/>
-      <c r="B17" s="309"/>
+      <c r="A17" s="269"/>
+      <c r="B17" s="270"/>
       <c r="C17" s="132"/>
-      <c r="D17" s="310"/>
+      <c r="D17" s="271"/>
       <c r="E17" s="132"/>
       <c r="F17" s="196">
         <f t="shared" si="0"/>
@@ -7841,10 +7850,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="308"/>
-      <c r="B18" s="309"/>
+      <c r="A18" s="269"/>
+      <c r="B18" s="270"/>
       <c r="C18" s="132"/>
-      <c r="D18" s="310"/>
+      <c r="D18" s="271"/>
       <c r="E18" s="132"/>
       <c r="F18" s="196">
         <f t="shared" si="0"/>
@@ -7852,10 +7861,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="308"/>
-      <c r="B19" s="309"/>
+      <c r="A19" s="269"/>
+      <c r="B19" s="270"/>
       <c r="C19" s="132"/>
-      <c r="D19" s="310"/>
+      <c r="D19" s="271"/>
       <c r="E19" s="132"/>
       <c r="F19" s="196">
         <f t="shared" si="0"/>
@@ -7863,10 +7872,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="308"/>
-      <c r="B20" s="309"/>
+      <c r="A20" s="269"/>
+      <c r="B20" s="270"/>
       <c r="C20" s="132"/>
-      <c r="D20" s="310"/>
+      <c r="D20" s="271"/>
       <c r="E20" s="132"/>
       <c r="F20" s="196">
         <f t="shared" si="0"/>
@@ -7874,10 +7883,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="308"/>
-      <c r="B21" s="309"/>
+      <c r="A21" s="269"/>
+      <c r="B21" s="270"/>
       <c r="C21" s="132"/>
-      <c r="D21" s="310"/>
+      <c r="D21" s="271"/>
       <c r="E21" s="132"/>
       <c r="F21" s="196">
         <f t="shared" si="0"/>
@@ -7885,10 +7894,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="308"/>
-      <c r="B22" s="309"/>
+      <c r="A22" s="269"/>
+      <c r="B22" s="270"/>
       <c r="C22" s="132"/>
-      <c r="D22" s="310"/>
+      <c r="D22" s="271"/>
       <c r="E22" s="132"/>
       <c r="F22" s="196">
         <f t="shared" si="0"/>
@@ -7896,10 +7905,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="308"/>
-      <c r="B23" s="309"/>
+      <c r="A23" s="269"/>
+      <c r="B23" s="270"/>
       <c r="C23" s="132"/>
-      <c r="D23" s="310"/>
+      <c r="D23" s="271"/>
       <c r="E23" s="132"/>
       <c r="F23" s="196">
         <f t="shared" si="0"/>
@@ -7907,10 +7916,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="308"/>
-      <c r="B24" s="309"/>
+      <c r="A24" s="269"/>
+      <c r="B24" s="270"/>
       <c r="C24" s="132"/>
-      <c r="D24" s="310"/>
+      <c r="D24" s="271"/>
       <c r="E24" s="132"/>
       <c r="F24" s="196">
         <f t="shared" si="0"/>
@@ -7919,10 +7928,10 @@
       <c r="G24" s="162"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="308"/>
-      <c r="B25" s="309"/>
+      <c r="A25" s="269"/>
+      <c r="B25" s="270"/>
       <c r="C25" s="132"/>
-      <c r="D25" s="310"/>
+      <c r="D25" s="271"/>
       <c r="E25" s="132"/>
       <c r="F25" s="196">
         <f t="shared" si="0"/>
@@ -7930,10 +7939,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="308"/>
-      <c r="B26" s="309"/>
+      <c r="A26" s="269"/>
+      <c r="B26" s="270"/>
       <c r="C26" s="132"/>
-      <c r="D26" s="310"/>
+      <c r="D26" s="271"/>
       <c r="E26" s="132"/>
       <c r="F26" s="196">
         <f t="shared" si="0"/>
@@ -7941,10 +7950,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="308"/>
-      <c r="B27" s="309"/>
+      <c r="A27" s="269"/>
+      <c r="B27" s="270"/>
       <c r="C27" s="132"/>
-      <c r="D27" s="310"/>
+      <c r="D27" s="271"/>
       <c r="E27" s="132"/>
       <c r="F27" s="196">
         <f t="shared" si="0"/>
@@ -7952,10 +7961,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="308"/>
-      <c r="B28" s="309"/>
+      <c r="A28" s="269"/>
+      <c r="B28" s="270"/>
       <c r="C28" s="132"/>
-      <c r="D28" s="310"/>
+      <c r="D28" s="271"/>
       <c r="E28" s="132"/>
       <c r="F28" s="196">
         <f t="shared" si="0"/>
@@ -7963,10 +7972,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="308"/>
-      <c r="B29" s="309"/>
+      <c r="A29" s="269"/>
+      <c r="B29" s="270"/>
       <c r="C29" s="132"/>
-      <c r="D29" s="310"/>
+      <c r="D29" s="271"/>
       <c r="E29" s="132"/>
       <c r="F29" s="196">
         <f t="shared" si="0"/>
@@ -7974,10 +7983,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="308"/>
-      <c r="B30" s="309"/>
+      <c r="A30" s="269"/>
+      <c r="B30" s="270"/>
       <c r="C30" s="132"/>
-      <c r="D30" s="308"/>
+      <c r="D30" s="269"/>
       <c r="E30" s="132"/>
       <c r="F30" s="196">
         <f t="shared" si="0"/>
@@ -7985,10 +7994,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="308"/>
-      <c r="B31" s="309"/>
+      <c r="A31" s="269"/>
+      <c r="B31" s="270"/>
       <c r="C31" s="132"/>
-      <c r="D31" s="310"/>
+      <c r="D31" s="271"/>
       <c r="E31" s="132"/>
       <c r="F31" s="196">
         <f t="shared" si="0"/>
@@ -7996,10 +8005,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="308"/>
-      <c r="B32" s="309"/>
+      <c r="A32" s="269"/>
+      <c r="B32" s="270"/>
       <c r="C32" s="132"/>
-      <c r="D32" s="310"/>
+      <c r="D32" s="271"/>
       <c r="E32" s="132"/>
       <c r="F32" s="196">
         <f t="shared" si="0"/>
@@ -8008,10 +8017,10 @@
       <c r="G32" s="162"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="308"/>
-      <c r="B33" s="309"/>
+      <c r="A33" s="269"/>
+      <c r="B33" s="270"/>
       <c r="C33" s="132"/>
-      <c r="D33" s="310"/>
+      <c r="D33" s="271"/>
       <c r="E33" s="132"/>
       <c r="F33" s="196">
         <f t="shared" si="0"/>
@@ -8019,10 +8028,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="308"/>
-      <c r="B34" s="309"/>
+      <c r="A34" s="269"/>
+      <c r="B34" s="270"/>
       <c r="C34" s="132"/>
-      <c r="D34" s="310"/>
+      <c r="D34" s="271"/>
       <c r="E34" s="132"/>
       <c r="F34" s="196">
         <f t="shared" si="0"/>
@@ -8030,10 +8039,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="308"/>
-      <c r="B35" s="309"/>
+      <c r="A35" s="269"/>
+      <c r="B35" s="270"/>
       <c r="C35" s="132"/>
-      <c r="D35" s="310"/>
+      <c r="D35" s="271"/>
       <c r="E35" s="132"/>
       <c r="F35" s="196">
         <f t="shared" si="0"/>
@@ -8041,10 +8050,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="308"/>
-      <c r="B36" s="309"/>
+      <c r="A36" s="269"/>
+      <c r="B36" s="270"/>
       <c r="C36" s="132"/>
-      <c r="D36" s="310"/>
+      <c r="D36" s="271"/>
       <c r="E36" s="132"/>
       <c r="F36" s="196">
         <f t="shared" si="0"/>
@@ -8052,10 +8061,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="308"/>
-      <c r="B37" s="309"/>
+      <c r="A37" s="269"/>
+      <c r="B37" s="270"/>
       <c r="C37" s="132"/>
-      <c r="D37" s="310"/>
+      <c r="D37" s="271"/>
       <c r="E37" s="132"/>
       <c r="F37" s="196">
         <f t="shared" si="0"/>
@@ -8063,10 +8072,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="308"/>
-      <c r="B38" s="309"/>
+      <c r="A38" s="269"/>
+      <c r="B38" s="270"/>
       <c r="C38" s="132"/>
-      <c r="D38" s="310"/>
+      <c r="D38" s="271"/>
       <c r="E38" s="132"/>
       <c r="F38" s="196">
         <f t="shared" si="0"/>
@@ -8074,10 +8083,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="308"/>
-      <c r="B39" s="309"/>
+      <c r="A39" s="269"/>
+      <c r="B39" s="270"/>
       <c r="C39" s="132"/>
-      <c r="D39" s="310"/>
+      <c r="D39" s="271"/>
       <c r="E39" s="132"/>
       <c r="F39" s="196">
         <f t="shared" si="0"/>
@@ -8085,10 +8094,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="308"/>
-      <c r="B40" s="309"/>
+      <c r="A40" s="269"/>
+      <c r="B40" s="270"/>
       <c r="C40" s="132"/>
-      <c r="D40" s="310"/>
+      <c r="D40" s="271"/>
       <c r="E40" s="86"/>
       <c r="F40" s="196">
         <f t="shared" si="0"/>
@@ -8096,10 +8105,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="308"/>
-      <c r="B41" s="309"/>
+      <c r="A41" s="269"/>
+      <c r="B41" s="270"/>
       <c r="C41" s="132"/>
-      <c r="D41" s="310"/>
+      <c r="D41" s="271"/>
       <c r="E41" s="86"/>
       <c r="F41" s="196">
         <f t="shared" si="0"/>
@@ -8107,10 +8116,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="310"/>
-      <c r="B42" s="311"/>
+      <c r="A42" s="271"/>
+      <c r="B42" s="272"/>
       <c r="C42" s="86"/>
-      <c r="D42" s="310"/>
+      <c r="D42" s="271"/>
       <c r="E42" s="86"/>
       <c r="F42" s="196">
         <f t="shared" si="0"/>
@@ -8680,10 +8689,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <sortState ref="B7:C9">
+    <sortCondition ref="B7:B9"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10497,23 +10511,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="292"/>
-      <c r="C1" s="294" t="s">
+      <c r="B1" s="274"/>
+      <c r="C1" s="276" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="293"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -10523,21 +10537,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="279"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="280"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="265" t="s">
+      <c r="R3" s="285" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10552,14 +10566,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="281" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="282"/>
+      <c r="H4" s="283" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="284"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -10569,11 +10583,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="272" t="s">
+      <c r="P4" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="273"/>
-      <c r="R4" s="266"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="286"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -12057,11 +12071,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="80"/>
-      <c r="M40" s="303">
+      <c r="M40" s="312">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="276">
+      <c r="N40" s="296">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -12087,8 +12101,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="275"/>
-      <c r="N41" s="277"/>
+      <c r="M41" s="295"/>
+      <c r="N41" s="297"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -12303,29 +12317,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="299"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="280">
+      <c r="K53" s="300">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="282">
+      <c r="L53" s="301"/>
+      <c r="M53" s="302">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="283"/>
+      <c r="N53" s="303"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="284" t="s">
+      <c r="D54" s="304" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="284"/>
+      <c r="E54" s="304"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -12336,22 +12350,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="285" t="s">
+      <c r="D55" s="305" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="285"/>
+      <c r="E55" s="305"/>
       <c r="F55" s="115">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="286" t="s">
+      <c r="I55" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="287"/>
-      <c r="K55" s="288">
+      <c r="J55" s="307"/>
+      <c r="K55" s="308">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="289"/>
+      <c r="L55" s="309"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -12382,11 +12396,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="290">
+      <c r="K57" s="310">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="291"/>
+      <c r="L57" s="311"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -12403,22 +12417,22 @@
       <c r="C59" s="133">
         <v>44619</v>
       </c>
-      <c r="D59" s="267" t="s">
+      <c r="D59" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="268"/>
+      <c r="E59" s="288"/>
       <c r="F59" s="134">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="269" t="s">
+      <c r="I59" s="289" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="270"/>
-      <c r="K59" s="271">
+      <c r="J59" s="290"/>
+      <c r="K59" s="291">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="271"/>
+      <c r="L59" s="291"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -12562,18 +12576,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -12583,6 +12585,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13887,23 +13901,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="292"/>
-      <c r="C1" s="294" t="s">
+      <c r="B1" s="274"/>
+      <c r="C1" s="276" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="293"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -13913,21 +13927,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="279"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="280"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="265" t="s">
+      <c r="R3" s="285" t="s">
         <v>38</v>
       </c>
     </row>
@@ -13942,14 +13956,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="281" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="282"/>
+      <c r="H4" s="283" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="284"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -13959,11 +13973,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="272" t="s">
+      <c r="P4" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="273"/>
-      <c r="R4" s="266"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="286"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -15431,11 +15445,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="274">
+      <c r="M40" s="294">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="276">
+      <c r="N40" s="296">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -15465,8 +15479,8 @@
       <c r="L41" s="75">
         <v>25678</v>
       </c>
-      <c r="M41" s="275"/>
-      <c r="N41" s="277"/>
+      <c r="M41" s="295"/>
+      <c r="N41" s="297"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -15681,29 +15695,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="299"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="280">
+      <c r="K53" s="300">
         <f>I51+L51</f>
         <v>82963.709999999992</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="282">
+      <c r="L53" s="301"/>
+      <c r="M53" s="302">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N53" s="283"/>
+      <c r="N53" s="303"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="284" t="s">
+      <c r="D54" s="304" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="284"/>
+      <c r="E54" s="304"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1831731.29</v>
@@ -15714,22 +15728,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="285" t="s">
+      <c r="D55" s="305" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="285"/>
+      <c r="E55" s="305"/>
       <c r="F55" s="115">
         <v>-1848136.64</v>
       </c>
-      <c r="I55" s="286" t="s">
+      <c r="I55" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="287"/>
-      <c r="K55" s="288">
+      <c r="J55" s="307"/>
+      <c r="K55" s="308">
         <f>F57+F58+F59</f>
         <v>203012.02000000014</v>
       </c>
-      <c r="L55" s="289"/>
+      <c r="L55" s="309"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -15760,11 +15774,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="290">
+      <c r="K57" s="310">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L57" s="291"/>
+      <c r="L57" s="311"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -15781,22 +15795,22 @@
       <c r="C59" s="133">
         <v>44647</v>
       </c>
-      <c r="D59" s="267" t="s">
+      <c r="D59" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="268"/>
+      <c r="E59" s="288"/>
       <c r="F59" s="134">
         <v>219417.37</v>
       </c>
-      <c r="I59" s="269" t="s">
+      <c r="I59" s="289" t="s">
         <v>226</v>
       </c>
-      <c r="J59" s="270"/>
-      <c r="K59" s="271">
+      <c r="J59" s="290"/>
+      <c r="K59" s="291">
         <f>K55+K57</f>
         <v>18669.830000000133</v>
       </c>
-      <c r="L59" s="271"/>
+      <c r="L59" s="291"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -15940,6 +15954,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -15949,18 +15975,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17411,8 +17425,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17435,23 +17449,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="292"/>
-      <c r="C1" s="294" t="s">
+      <c r="B1" s="274"/>
+      <c r="C1" s="276" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="293"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -17461,21 +17475,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="279"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="280"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="265" t="s">
+      <c r="R3" s="285" t="s">
         <v>38</v>
       </c>
     </row>
@@ -17490,14 +17504,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="281" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="282"/>
+      <c r="H4" s="283" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="284"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -17507,11 +17521,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="272" t="s">
+      <c r="P4" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="273"/>
-      <c r="R4" s="266"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="286"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -19154,11 +19168,11 @@
       <c r="L40" s="75">
         <v>30225</v>
       </c>
-      <c r="M40" s="274">
+      <c r="M40" s="294">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="276">
+      <c r="N40" s="296">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -19184,8 +19198,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="246"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="275"/>
-      <c r="N41" s="277"/>
+      <c r="M41" s="295"/>
+      <c r="N41" s="297"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -19400,29 +19414,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="299"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="280">
+      <c r="K53" s="300">
         <f>I51+L51</f>
         <v>86124</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="282">
+      <c r="L53" s="301"/>
+      <c r="M53" s="302">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="283"/>
+      <c r="N53" s="303"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="284" t="s">
+      <c r="D54" s="304" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="284"/>
+      <c r="E54" s="304"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>2185028</v>
@@ -19433,22 +19447,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="285" t="s">
+      <c r="D55" s="305" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="285"/>
+      <c r="E55" s="305"/>
       <c r="F55" s="115">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="286" t="s">
+      <c r="I55" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="287"/>
-      <c r="K55" s="288">
+      <c r="J55" s="307"/>
+      <c r="K55" s="308">
         <f>F57+F58+F59</f>
         <v>266670.11000000004</v>
       </c>
-      <c r="L55" s="289"/>
+      <c r="L55" s="309"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -19479,11 +19493,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="290">
+      <c r="K57" s="310">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="291"/>
+      <c r="L57" s="311"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -19500,20 +19514,20 @@
       <c r="C59" s="133">
         <v>44682</v>
       </c>
-      <c r="D59" s="267" t="s">
+      <c r="D59" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="268"/>
+      <c r="E59" s="288"/>
       <c r="F59" s="134">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="269"/>
-      <c r="J59" s="270"/>
-      <c r="K59" s="271">
+      <c r="I59" s="289"/>
+      <c r="J59" s="290"/>
+      <c r="K59" s="291">
         <f>K55+K57</f>
         <v>47252.740000000049</v>
       </c>
-      <c r="L59" s="271"/>
+      <c r="L59" s="291"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -19657,6 +19671,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -19666,18 +19692,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -21132,8 +21146,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21156,23 +21170,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="292"/>
-      <c r="C1" s="294" t="s">
+      <c r="B1" s="274"/>
+      <c r="C1" s="276" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="293"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -21182,21 +21196,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="279"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="280"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="265" t="s">
+      <c r="R3" s="285" t="s">
         <v>38</v>
       </c>
     </row>
@@ -21211,14 +21225,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="281" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="282"/>
+      <c r="H4" s="283" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="284"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -21228,11 +21242,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="272" t="s">
+      <c r="P4" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="273"/>
-      <c r="R4" s="266"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="286"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -21377,37 +21391,45 @@
         <v>44686</v>
       </c>
       <c r="C8" s="26">
-        <v>0</v>
-      </c>
-      <c r="D8" s="41"/>
+        <v>1360</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="E8" s="28">
         <v>44686</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="29">
+        <v>58940</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="30">
         <v>44686</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="31">
+        <v>28</v>
+      </c>
       <c r="J8" s="44"/>
       <c r="K8" s="45"/>
       <c r="L8" s="40"/>
       <c r="M8" s="32">
-        <v>0</v>
+        <f>52916+15000</f>
+        <v>67916</v>
       </c>
       <c r="N8" s="33">
-        <v>0</v>
+        <v>897</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70201</v>
       </c>
       <c r="Q8" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="184">
+        <v>11261</v>
+      </c>
       <c r="S8">
         <v>9</v>
       </c>
@@ -21424,17 +21446,22 @@
       <c r="E9" s="28">
         <v>44687</v>
       </c>
-      <c r="F9" s="29"/>
+      <c r="F9" s="29">
+        <v>98700</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="30">
         <v>44687</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="31">
+        <v>85</v>
+      </c>
       <c r="J9" s="38"/>
       <c r="K9" s="46"/>
       <c r="L9" s="40"/>
       <c r="M9" s="32">
-        <v>0</v>
+        <f>20000+40000+38615</f>
+        <v>98615</v>
       </c>
       <c r="N9" s="33">
         <v>0</v>
@@ -21442,7 +21469,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="34">
         <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
+        <v>98700</v>
       </c>
       <c r="Q9" s="13">
         <f t="shared" si="1"/>
@@ -21459,31 +21486,38 @@
         <v>44688</v>
       </c>
       <c r="C10" s="26">
-        <v>0</v>
-      </c>
-      <c r="D10" s="36"/>
+        <v>7184</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="28">
         <v>44688</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="29">
+        <v>102747</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="30">
         <v>44688</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="31">
+        <v>60</v>
+      </c>
       <c r="J10" s="38"/>
       <c r="K10" s="47"/>
       <c r="L10" s="48"/>
       <c r="M10" s="32">
-        <v>0</v>
+        <f>40000+47403</f>
+        <v>87403</v>
       </c>
       <c r="N10" s="33">
-        <v>0</v>
+        <v>8100</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>102747</v>
       </c>
       <c r="Q10" s="13">
         <f t="shared" si="1"/>
@@ -21503,31 +21537,44 @@
         <v>44689</v>
       </c>
       <c r="C11" s="26">
-        <v>0</v>
-      </c>
-      <c r="D11" s="36"/>
+        <v>5204</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="E11" s="28">
         <v>44689</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="29">
+        <v>114024</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="30">
         <v>44689</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="40"/>
+      <c r="I11" s="31">
+        <v>22</v>
+      </c>
+      <c r="J11" s="44">
+        <v>44689</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="L11" s="40">
+        <v>9717</v>
+      </c>
       <c r="M11" s="32">
-        <v>0</v>
+        <f>80000+18221</f>
+        <v>98221</v>
       </c>
       <c r="N11" s="33">
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="34">
         <f>N11+M11+L11+I11+C11</f>
-        <v>0</v>
+        <v>114024</v>
       </c>
       <c r="Q11" s="13">
         <f>P11-F11</f>
@@ -21546,35 +21593,42 @@
         <v>44690</v>
       </c>
       <c r="C12" s="26">
-        <v>0</v>
-      </c>
-      <c r="D12" s="36"/>
+        <v>2800</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="E12" s="28">
         <v>44690</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="29">
+        <v>85296</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="30">
         <v>44690</v>
       </c>
-      <c r="I12" s="31"/>
+      <c r="I12" s="31">
+        <v>39</v>
+      </c>
       <c r="J12" s="38"/>
       <c r="K12" s="50"/>
       <c r="L12" s="40"/>
       <c r="M12" s="32">
-        <v>0</v>
+        <f>57065+24240+200</f>
+        <v>81505</v>
       </c>
       <c r="N12" s="33">
-        <v>0</v>
+        <v>1152</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>85496</v>
       </c>
       <c r="Q12" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="R12" s="8"/>
       <c r="S12">
@@ -21587,31 +21641,38 @@
         <v>44691</v>
       </c>
       <c r="C13" s="26">
-        <v>0</v>
-      </c>
-      <c r="D13" s="41"/>
+        <v>800</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="E13" s="28">
         <v>44691</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="29">
+        <v>92517</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="30">
         <v>44691</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="31">
+        <v>19</v>
+      </c>
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
       <c r="M13" s="32">
-        <v>0</v>
+        <f>20000+40000+31098</f>
+        <v>91098</v>
       </c>
       <c r="N13" s="33">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>92517</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" si="1"/>
@@ -21634,25 +21695,29 @@
       <c r="E14" s="28">
         <v>44692</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="29">
+        <v>35612</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="30">
         <v>44692</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="31">
+        <v>309</v>
+      </c>
       <c r="J14" s="38"/>
       <c r="K14" s="45"/>
       <c r="L14" s="40"/>
       <c r="M14" s="32">
-        <v>0</v>
+        <v>35029</v>
       </c>
       <c r="N14" s="33">
-        <v>0</v>
+        <v>274</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35612</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="1"/>
@@ -21669,30 +21734,37 @@
         <v>44693</v>
       </c>
       <c r="C15" s="26">
-        <v>0</v>
-      </c>
-      <c r="D15" s="51"/>
+        <v>18388</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" s="28">
         <v>44693</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="29">
+        <v>69146</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="30">
         <v>44693</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="31">
+        <v>90</v>
+      </c>
       <c r="J15" s="38"/>
       <c r="K15" s="45"/>
       <c r="L15" s="40"/>
       <c r="M15" s="32">
-        <v>0</v>
+        <f>30668+20000</f>
+        <v>50668</v>
       </c>
       <c r="N15" s="33">
         <v>0</v>
       </c>
       <c r="P15" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69146</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" si="1"/>
@@ -21715,24 +21787,29 @@
       <c r="E16" s="28">
         <v>44694</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="29">
+        <v>98563</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="30">
         <v>44694</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="31">
+        <v>220</v>
+      </c>
       <c r="J16" s="38"/>
       <c r="K16" s="45"/>
       <c r="L16" s="9"/>
       <c r="M16" s="32">
-        <v>0</v>
+        <f>63232+25000</f>
+        <v>88232</v>
       </c>
       <c r="N16" s="33">
-        <v>0</v>
+        <v>10111</v>
       </c>
       <c r="P16" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98563</v>
       </c>
       <c r="Q16" s="13">
         <f t="shared" si="1"/>
@@ -21751,30 +21828,43 @@
         <v>44695</v>
       </c>
       <c r="C17" s="26">
-        <v>0</v>
-      </c>
-      <c r="D17" s="41"/>
+        <v>1411</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>279</v>
+      </c>
       <c r="E17" s="28">
         <v>44695</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="29">
+        <v>149845</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="30">
         <v>44695</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="48"/>
+      <c r="I17" s="31">
+        <v>364</v>
+      </c>
+      <c r="J17" s="38">
+        <v>44695</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>280</v>
+      </c>
+      <c r="L17" s="48">
+        <v>11900</v>
+      </c>
       <c r="M17" s="32">
-        <v>0</v>
+        <f>12366+41750+45477+25000</f>
+        <v>124593</v>
       </c>
       <c r="N17" s="33">
-        <v>0</v>
+        <v>11577</v>
       </c>
       <c r="P17" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149845</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" si="1"/>
@@ -21797,24 +21887,29 @@
       <c r="E18" s="28">
         <v>44696</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="29">
+        <v>122601</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="30">
         <v>44696</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="31">
+        <v>0</v>
+      </c>
       <c r="J18" s="38"/>
       <c r="K18" s="53"/>
       <c r="L18" s="40"/>
       <c r="M18" s="32">
-        <v>0</v>
+        <f>95000+26901</f>
+        <v>121901</v>
       </c>
       <c r="N18" s="33">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="P18" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>122601</v>
       </c>
       <c r="Q18" s="13">
         <f t="shared" si="1"/>
@@ -21837,29 +21932,34 @@
       <c r="E19" s="28">
         <v>44697</v>
       </c>
-      <c r="F19" s="29"/>
+      <c r="F19" s="29">
+        <v>62516</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="30">
         <v>44697</v>
       </c>
-      <c r="I19" s="31"/>
+      <c r="I19" s="31">
+        <v>59</v>
+      </c>
       <c r="J19" s="38"/>
       <c r="K19" s="54"/>
       <c r="L19" s="55"/>
       <c r="M19" s="32">
-        <v>0</v>
+        <f>22000+39329</f>
+        <v>61329</v>
       </c>
       <c r="N19" s="33">
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62518</v>
       </c>
       <c r="Q19" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19" s="8"/>
       <c r="S19">
@@ -21878,24 +21978,29 @@
       <c r="E20" s="28">
         <v>44698</v>
       </c>
-      <c r="F20" s="29"/>
+      <c r="F20" s="29">
+        <v>87181</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="30">
         <v>44698</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="31">
+        <v>48</v>
+      </c>
       <c r="J20" s="38"/>
       <c r="K20" s="56"/>
       <c r="L20" s="48"/>
       <c r="M20" s="32">
-        <v>0</v>
+        <f>36535+50000</f>
+        <v>86535</v>
       </c>
       <c r="N20" s="33">
-        <v>0</v>
+        <v>598</v>
       </c>
       <c r="P20" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>87181</v>
       </c>
       <c r="Q20" s="13">
         <f t="shared" si="1"/>
@@ -21912,30 +22017,37 @@
         <v>44699</v>
       </c>
       <c r="C21" s="26">
-        <v>0</v>
-      </c>
-      <c r="D21" s="36"/>
+        <v>2100</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="E21" s="28">
         <v>44699</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="29">
+        <v>43454</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="30">
         <v>44699</v>
       </c>
-      <c r="I21" s="31"/>
+      <c r="I21" s="31">
+        <v>90</v>
+      </c>
       <c r="J21" s="38"/>
       <c r="K21" s="57"/>
       <c r="L21" s="48"/>
       <c r="M21" s="32">
-        <v>0</v>
+        <f>31220+10000</f>
+        <v>41220</v>
       </c>
       <c r="N21" s="33">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="P21" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43454</v>
       </c>
       <c r="Q21" s="13">
         <f t="shared" si="1"/>
@@ -22595,23 +22707,23 @@
       <c r="H40" s="37"/>
       <c r="I40" s="88"/>
       <c r="J40" s="73"/>
-      <c r="K40" s="312"/>
+      <c r="K40" s="273"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="274">
+      <c r="M40" s="294">
         <f>SUM(M5:M39)</f>
-        <v>169416</v>
-      </c>
-      <c r="N40" s="276">
+        <v>1303681</v>
+      </c>
+      <c r="N40" s="296">
         <f>SUM(N5:N39)</f>
-        <v>1374</v>
+        <v>37417</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>171045</v>
+        <v>1403650</v>
       </c>
       <c r="Q40" s="13">
         <f t="shared" si="1"/>
-        <v>171045</v>
+        <v>1403650</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22627,8 +22739,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="246"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="275"/>
-      <c r="N41" s="277"/>
+      <c r="M41" s="295"/>
+      <c r="N41" s="297"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -22801,7 +22913,7 @@
       </c>
       <c r="C51" s="106">
         <f>SUM(C5:C50)</f>
-        <v>0</v>
+        <v>39247</v>
       </c>
       <c r="D51" s="107"/>
       <c r="E51" s="108" t="s">
@@ -22809,7 +22921,7 @@
       </c>
       <c r="F51" s="109">
         <f>SUM(F5:F50)</f>
-        <v>171044</v>
+        <v>1392186</v>
       </c>
       <c r="G51" s="107"/>
       <c r="H51" s="110" t="s">
@@ -22817,7 +22929,7 @@
       </c>
       <c r="I51" s="111">
         <f>SUM(I5:I50)</f>
-        <v>255</v>
+        <v>1688</v>
       </c>
       <c r="J51" s="112"/>
       <c r="K51" s="113" t="s">
@@ -22825,7 +22937,7 @@
       </c>
       <c r="L51" s="114">
         <f>SUM(L5:L50)</f>
-        <v>0</v>
+        <v>21617</v>
       </c>
       <c r="M51" s="115"/>
       <c r="N51" s="115"/>
@@ -22843,32 +22955,32 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="299"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="280">
+      <c r="K53" s="300">
         <f>I51+L51</f>
-        <v>255</v>
-      </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="282">
+        <v>23305</v>
+      </c>
+      <c r="L53" s="301"/>
+      <c r="M53" s="302">
         <f>N40+M40</f>
-        <v>170790</v>
-      </c>
-      <c r="N53" s="283"/>
+        <v>1341098</v>
+      </c>
+      <c r="N53" s="303"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="284" t="s">
+      <c r="D54" s="304" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="284"/>
+      <c r="E54" s="304"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>170789</v>
+        <v>1329634</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -22876,22 +22988,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="285" t="s">
+      <c r="D55" s="305" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="285"/>
+      <c r="E55" s="305"/>
       <c r="F55" s="115">
         <v>0</v>
       </c>
-      <c r="I55" s="286" t="s">
+      <c r="I55" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="287"/>
-      <c r="K55" s="288">
+      <c r="J55" s="307"/>
+      <c r="K55" s="308">
         <f>F57+F58+F59</f>
-        <v>170789</v>
-      </c>
-      <c r="L55" s="289"/>
+        <v>1329634</v>
+      </c>
+      <c r="L55" s="309"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -22915,18 +23027,18 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>170789</v>
+        <v>1329634</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="290">
+      <c r="K57" s="310">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="291"/>
+      <c r="L57" s="311"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -22941,20 +23053,20 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="133"/>
-      <c r="D59" s="267" t="s">
+      <c r="D59" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="268"/>
+      <c r="E59" s="288"/>
       <c r="F59" s="134">
         <v>0</v>
       </c>
-      <c r="I59" s="269"/>
-      <c r="J59" s="270"/>
-      <c r="K59" s="271">
+      <c r="I59" s="289"/>
+      <c r="J59" s="290"/>
+      <c r="K59" s="291">
         <f>K55+K57</f>
-        <v>-127085.59000000003</v>
-      </c>
-      <c r="L59" s="271"/>
+        <v>1031759.4099999999</v>
+      </c>
+      <c r="L59" s="291"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -23098,6 +23210,20 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="M53:N53"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
@@ -23105,20 +23231,6 @@
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 27 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="312">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1257,6 +1257,9 @@
   </si>
   <si>
     <t>23292 C</t>
+  </si>
+  <si>
+    <t>NOMINA # 21</t>
   </si>
 </sst>
 </file>
@@ -7725,7 +7728,7 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -21416,8 +21419,11 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView topLeftCell="J3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="J17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22340,24 +22346,29 @@
       <c r="E22" s="28">
         <v>44700</v>
       </c>
-      <c r="F22" s="29"/>
+      <c r="F22" s="29">
+        <v>65355</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="30">
         <v>44700</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="31">
+        <v>56</v>
+      </c>
       <c r="J22" s="38"/>
       <c r="K22" s="45"/>
       <c r="L22" s="58"/>
       <c r="M22" s="32">
-        <v>0</v>
+        <f>30000+35299</f>
+        <v>65299</v>
       </c>
       <c r="N22" s="33">
         <v>0</v>
       </c>
       <c r="P22" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>65355</v>
       </c>
       <c r="Q22" s="13">
         <f t="shared" si="1"/>
@@ -22374,30 +22385,37 @@
         <v>44701</v>
       </c>
       <c r="C23" s="26">
-        <v>0</v>
-      </c>
-      <c r="D23" s="36"/>
+        <v>19197</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="28">
         <v>44701</v>
       </c>
-      <c r="F23" s="29"/>
+      <c r="F23" s="29">
+        <v>86439</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="30">
         <v>44701</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="31">
+        <v>169</v>
+      </c>
       <c r="J23" s="59"/>
       <c r="K23" s="60"/>
       <c r="L23" s="48"/>
       <c r="M23" s="32">
-        <v>0</v>
+        <f>30000+36609</f>
+        <v>66609</v>
       </c>
       <c r="N23" s="33">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="P23" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>86439</v>
       </c>
       <c r="Q23" s="13">
         <f t="shared" si="1"/>
@@ -22414,34 +22432,47 @@
         <v>44702</v>
       </c>
       <c r="C24" s="26">
-        <v>0</v>
-      </c>
-      <c r="D24" s="41"/>
+        <v>15</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" s="28">
         <v>44702</v>
       </c>
-      <c r="F24" s="29"/>
+      <c r="F24" s="29">
+        <v>91965</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="30">
         <v>44702</v>
       </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="63"/>
+      <c r="I24" s="31">
+        <v>60</v>
+      </c>
+      <c r="J24" s="181">
+        <v>44702</v>
+      </c>
+      <c r="K24" s="62" t="s">
+        <v>311</v>
+      </c>
+      <c r="L24" s="63">
+        <v>10800</v>
+      </c>
       <c r="M24" s="32">
-        <v>0</v>
+        <f>44952+5623+20000</f>
+        <v>70575</v>
       </c>
       <c r="N24" s="33">
-        <v>0</v>
+        <v>10516</v>
       </c>
       <c r="P24" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>91966</v>
       </c>
       <c r="Q24" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="8"/>
       <c r="S24">
@@ -22460,31 +22491,36 @@
       <c r="E25" s="28">
         <v>44703</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="29">
+        <v>118336</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="30">
         <v>44703</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="31">
+        <v>0</v>
+      </c>
       <c r="J25" s="64"/>
       <c r="K25" s="65"/>
       <c r="L25" s="66"/>
       <c r="M25" s="32">
-        <v>0</v>
+        <f>100000+14710</f>
+        <v>114710</v>
       </c>
       <c r="N25" s="33">
-        <v>0</v>
+        <v>3628</v>
       </c>
       <c r="O25" t="s">
         <v>8</v>
       </c>
       <c r="P25" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>118338</v>
       </c>
       <c r="Q25" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R25" s="8"/>
       <c r="S25">
@@ -22503,24 +22539,29 @@
       <c r="E26" s="28">
         <v>44704</v>
       </c>
-      <c r="F26" s="29"/>
+      <c r="F26" s="29">
+        <v>50361</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="30">
         <v>44704</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="31">
+        <v>53</v>
+      </c>
       <c r="J26" s="38"/>
       <c r="K26" s="62"/>
       <c r="L26" s="48"/>
       <c r="M26" s="32">
-        <v>0</v>
+        <f>44308+6000</f>
+        <v>50308</v>
       </c>
       <c r="N26" s="33">
         <v>0</v>
       </c>
       <c r="P26" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50361</v>
       </c>
       <c r="Q26" s="13">
         <f t="shared" si="1"/>
@@ -22981,19 +23022,19 @@
       <c r="L40" s="75"/>
       <c r="M40" s="283">
         <f>SUM(M5:M39)</f>
-        <v>1303681</v>
+        <v>1671182</v>
       </c>
       <c r="N40" s="285">
         <f>SUM(N5:N39)</f>
-        <v>37417</v>
+        <v>52025</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>1403650</v>
+        <v>1816109</v>
       </c>
       <c r="Q40" s="13">
         <f t="shared" si="1"/>
-        <v>1403650</v>
+        <v>1816109</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23183,7 +23224,7 @@
       </c>
       <c r="C51" s="106">
         <f>SUM(C5:C50)</f>
-        <v>39247</v>
+        <v>58459</v>
       </c>
       <c r="D51" s="107"/>
       <c r="E51" s="108" t="s">
@@ -23191,7 +23232,7 @@
       </c>
       <c r="F51" s="109">
         <f>SUM(F5:F50)</f>
-        <v>1392186</v>
+        <v>1804642</v>
       </c>
       <c r="G51" s="107"/>
       <c r="H51" s="110" t="s">
@@ -23199,7 +23240,7 @@
       </c>
       <c r="I51" s="111">
         <f>SUM(I5:I50)</f>
-        <v>1688</v>
+        <v>2026</v>
       </c>
       <c r="J51" s="112"/>
       <c r="K51" s="113" t="s">
@@ -23207,7 +23248,7 @@
       </c>
       <c r="L51" s="114">
         <f>SUM(L5:L50)</f>
-        <v>21617</v>
+        <v>32417</v>
       </c>
       <c r="M51" s="115"/>
       <c r="N51" s="115"/>
@@ -23232,12 +23273,12 @@
       <c r="J53" s="119"/>
       <c r="K53" s="289">
         <f>I51+L51</f>
-        <v>23305</v>
+        <v>34443</v>
       </c>
       <c r="L53" s="290"/>
       <c r="M53" s="291">
         <f>N40+M40</f>
-        <v>1341098</v>
+        <v>1723207</v>
       </c>
       <c r="N53" s="292"/>
       <c r="P53" s="34"/>
@@ -23250,7 +23291,7 @@
       <c r="E54" s="293"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>1329634</v>
+        <v>1711740</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -23271,7 +23312,7 @@
       <c r="J55" s="296"/>
       <c r="K55" s="297">
         <f>F57+F58+F59</f>
-        <v>1329634</v>
+        <v>1711740</v>
       </c>
       <c r="L55" s="298"/>
       <c r="P55" s="34"/>
@@ -23297,7 +23338,7 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>1329634</v>
+        <v>1711740</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
@@ -23334,7 +23375,7 @@
       <c r="J59" s="279"/>
       <c r="K59" s="280">
         <f>K55+K57</f>
-        <v>1031759.4099999999</v>
+        <v>1413865.41</v>
       </c>
       <c r="L59" s="280"/>
     </row>

</xml_diff>

<commit_message>
CIERRE 7 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/BALANCE   HERRADURA  MAYO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="324">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1290,6 +1290,12 @@
   </si>
   <si>
     <t>xxxxxxxxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEGURO </t>
+  </si>
+  <si>
+    <t>SEGURO</t>
   </si>
 </sst>
 </file>
@@ -2570,7 +2576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="319">
+  <cellXfs count="322">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3074,38 +3080,8 @@
     <xf numFmtId="44" fontId="2" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="17" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="27" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3188,17 +3164,54 @@
     <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="27" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5648,23 +5661,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="277"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="305"/>
+      <c r="C1" s="307" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="278"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -5674,21 +5687,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="281" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="282"/>
+      <c r="B3" s="309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="310"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="311" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="283"/>
+      <c r="I3" s="311"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="288" t="s">
+      <c r="R3" s="278" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5703,14 +5716,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="284" t="s">
+      <c r="E4" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="H4" s="286" t="s">
+      <c r="F4" s="313"/>
+      <c r="H4" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="287"/>
+      <c r="I4" s="315"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -5720,11 +5733,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="295" t="s">
+      <c r="P4" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="289"/>
+      <c r="Q4" s="286"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -7225,11 +7238,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="297">
+      <c r="M40" s="287">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="299">
+      <c r="N40" s="289">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -7255,8 +7268,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="298"/>
-      <c r="N41" s="300"/>
+      <c r="M41" s="288"/>
+      <c r="N41" s="290"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -7471,29 +7484,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="301" t="s">
+      <c r="H53" s="291" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="302"/>
+      <c r="I53" s="292"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="303">
+      <c r="K53" s="293">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="304"/>
-      <c r="M53" s="305">
+      <c r="L53" s="294"/>
+      <c r="M53" s="295">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="306"/>
+      <c r="N53" s="296"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="307" t="s">
+      <c r="D54" s="297" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="307"/>
+      <c r="E54" s="297"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -7504,22 +7517,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="308" t="s">
+      <c r="D55" s="298" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="308"/>
+      <c r="E55" s="298"/>
       <c r="F55" s="115">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="309" t="s">
+      <c r="I55" s="299" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="310"/>
-      <c r="K55" s="311">
+      <c r="J55" s="300"/>
+      <c r="K55" s="301">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="312"/>
+      <c r="L55" s="302"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -7550,11 +7563,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="313">
+      <c r="K57" s="303">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="314"/>
+      <c r="L57" s="304"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -7571,22 +7584,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="290" t="s">
+      <c r="D59" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="291"/>
+      <c r="E59" s="281"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="292" t="s">
+      <c r="I59" s="282" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="293"/>
-      <c r="K59" s="294">
+      <c r="J59" s="283"/>
+      <c r="K59" s="284">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="294"/>
+      <c r="L59" s="284"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -7730,6 +7743,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -7745,12 +7764,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10840,23 +10853,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="277"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="305"/>
+      <c r="C1" s="307" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="278"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -10866,21 +10879,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="281" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="282"/>
+      <c r="B3" s="309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="310"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="311" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="283"/>
+      <c r="I3" s="311"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="288" t="s">
+      <c r="R3" s="278" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10895,14 +10908,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="284" t="s">
+      <c r="E4" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="H4" s="286" t="s">
+      <c r="F4" s="313"/>
+      <c r="H4" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="287"/>
+      <c r="I4" s="315"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -10912,11 +10925,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="295" t="s">
+      <c r="P4" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="289"/>
+      <c r="Q4" s="286"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -12400,11 +12413,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="80"/>
-      <c r="M40" s="315">
+      <c r="M40" s="316">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="299">
+      <c r="N40" s="289">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -12430,8 +12443,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="298"/>
-      <c r="N41" s="300"/>
+      <c r="M41" s="288"/>
+      <c r="N41" s="290"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -12646,29 +12659,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="301" t="s">
+      <c r="H53" s="291" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="302"/>
+      <c r="I53" s="292"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="303">
+      <c r="K53" s="293">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="304"/>
-      <c r="M53" s="305">
+      <c r="L53" s="294"/>
+      <c r="M53" s="295">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="306"/>
+      <c r="N53" s="296"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="307" t="s">
+      <c r="D54" s="297" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="307"/>
+      <c r="E54" s="297"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -12679,22 +12692,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="308" t="s">
+      <c r="D55" s="298" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="308"/>
+      <c r="E55" s="298"/>
       <c r="F55" s="115">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="309" t="s">
+      <c r="I55" s="299" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="310"/>
-      <c r="K55" s="311">
+      <c r="J55" s="300"/>
+      <c r="K55" s="301">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="312"/>
+      <c r="L55" s="302"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -12725,11 +12738,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="313">
+      <c r="K57" s="303">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="314"/>
+      <c r="L57" s="304"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -12746,22 +12759,22 @@
       <c r="C59" s="133">
         <v>44619</v>
       </c>
-      <c r="D59" s="290" t="s">
+      <c r="D59" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="291"/>
+      <c r="E59" s="281"/>
       <c r="F59" s="134">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="292" t="s">
+      <c r="I59" s="282" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="293"/>
-      <c r="K59" s="294">
+      <c r="J59" s="283"/>
+      <c r="K59" s="284">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="294"/>
+      <c r="L59" s="284"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -12905,6 +12918,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -12914,18 +12939,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14207,7 +14220,7 @@
   <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14230,23 +14243,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="277"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="305"/>
+      <c r="C1" s="307" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="278"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14256,21 +14269,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="281" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="282"/>
+      <c r="B3" s="309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="310"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="311" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="283"/>
+      <c r="I3" s="311"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="288" t="s">
+      <c r="R3" s="278" t="s">
         <v>38</v>
       </c>
     </row>
@@ -14285,14 +14298,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="284" t="s">
+      <c r="E4" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="H4" s="286" t="s">
+      <c r="F4" s="313"/>
+      <c r="H4" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="287"/>
+      <c r="I4" s="315"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -14302,11 +14315,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="295" t="s">
+      <c r="P4" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="289"/>
+      <c r="Q4" s="286"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -15601,13 +15614,13 @@
       <c r="H34" s="30"/>
       <c r="I34" s="31"/>
       <c r="J34" s="73">
-        <v>44629</v>
-      </c>
-      <c r="K34" s="81" t="s">
-        <v>317</v>
-      </c>
-      <c r="L34" s="82">
-        <v>3133.5</v>
+        <v>44627</v>
+      </c>
+      <c r="K34" s="317" t="s">
+        <v>322</v>
+      </c>
+      <c r="L34" s="320">
+        <v>1195.68</v>
       </c>
       <c r="M34" s="32">
         <v>0</v>
@@ -15617,11 +15630,11 @@
       </c>
       <c r="P34" s="34">
         <f t="shared" si="0"/>
-        <v>3133.5</v>
+        <v>1195.68</v>
       </c>
       <c r="Q34" s="13">
         <f t="shared" si="1"/>
-        <v>3133.5</v>
+        <v>1195.68</v>
       </c>
       <c r="R34" s="8"/>
     </row>
@@ -15636,13 +15649,13 @@
       <c r="H35" s="30"/>
       <c r="I35" s="31"/>
       <c r="J35" s="73">
-        <v>44645</v>
-      </c>
-      <c r="K35" s="76" t="s">
-        <v>318</v>
+        <v>44629</v>
+      </c>
+      <c r="K35" s="221" t="s">
+        <v>317</v>
       </c>
       <c r="L35" s="80">
-        <v>1392</v>
+        <v>3133.5</v>
       </c>
       <c r="M35" s="220">
         <v>0</v>
@@ -15652,11 +15665,11 @@
       </c>
       <c r="P35" s="34">
         <f t="shared" si="0"/>
-        <v>1392</v>
+        <v>3133.5</v>
       </c>
       <c r="Q35" s="13">
         <f t="shared" si="1"/>
-        <v>1392</v>
+        <v>3133.5</v>
       </c>
       <c r="R35" s="8"/>
     </row>
@@ -15671,13 +15684,13 @@
       <c r="H36" s="30"/>
       <c r="I36" s="31"/>
       <c r="J36" s="73">
-        <v>44649</v>
-      </c>
-      <c r="K36" s="316" t="s">
-        <v>319</v>
+        <v>44645</v>
+      </c>
+      <c r="K36" s="319" t="s">
+        <v>318</v>
       </c>
       <c r="L36" s="80">
-        <v>1749.14</v>
+        <v>1392</v>
       </c>
       <c r="M36" s="220">
         <v>0</v>
@@ -15687,11 +15700,11 @@
       </c>
       <c r="P36" s="34">
         <f t="shared" si="0"/>
-        <v>1749.14</v>
+        <v>1392</v>
       </c>
       <c r="Q36" s="13">
         <f t="shared" si="1"/>
-        <v>1749.14</v>
+        <v>1392</v>
       </c>
       <c r="R36" s="8"/>
     </row>
@@ -15705,9 +15718,15 @@
       <c r="G37" s="2"/>
       <c r="H37" s="30"/>
       <c r="I37" s="31"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="317"/>
-      <c r="L37" s="80"/>
+      <c r="J37" s="73">
+        <v>44649</v>
+      </c>
+      <c r="K37" s="318" t="s">
+        <v>319</v>
+      </c>
+      <c r="L37" s="80">
+        <v>1749.14</v>
+      </c>
       <c r="M37" s="220">
         <v>0</v>
       </c>
@@ -15716,11 +15735,11 @@
       </c>
       <c r="P37" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1749.14</v>
       </c>
       <c r="Q37" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1749.14</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15736,7 +15755,7 @@
       <c r="J38" s="73">
         <v>44649</v>
       </c>
-      <c r="K38" s="76" t="s">
+      <c r="K38" s="321" t="s">
         <v>190</v>
       </c>
       <c r="L38" s="80">
@@ -15798,21 +15817,21 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="297">
+      <c r="M40" s="287">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="299">
+      <c r="N40" s="289">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>2013409.3499999999</v>
+        <v>2014605.0299999998</v>
       </c>
       <c r="Q40" s="13">
         <f t="shared" si="1"/>
-        <v>2013409.3499999999</v>
+        <v>2014605.0299999998</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15828,8 +15847,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="245"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="298"/>
-      <c r="N41" s="300"/>
+      <c r="M41" s="288"/>
+      <c r="N41" s="290"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -15954,7 +15973,7 @@
       </c>
       <c r="L47" s="114">
         <f>SUM(L5:L46)</f>
-        <v>85538.35</v>
+        <v>86734.03</v>
       </c>
       <c r="M47" s="115"/>
       <c r="N47" s="115"/>
@@ -15972,32 +15991,32 @@
       <c r="A49" s="117"/>
       <c r="B49" s="118"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="301" t="s">
+      <c r="H49" s="291" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="302"/>
+      <c r="I49" s="292"/>
       <c r="J49" s="119"/>
-      <c r="K49" s="303">
+      <c r="K49" s="293">
         <f>I47+L47</f>
-        <v>89238.35</v>
-      </c>
-      <c r="L49" s="304"/>
-      <c r="M49" s="305">
+        <v>90434.03</v>
+      </c>
+      <c r="L49" s="294"/>
+      <c r="M49" s="295">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="306"/>
+      <c r="N49" s="296"/>
       <c r="P49" s="34"/>
       <c r="Q49" s="9"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="307" t="s">
+      <c r="D50" s="297" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="307"/>
+      <c r="E50" s="297"/>
       <c r="F50" s="120">
         <f>F47-K49-C47</f>
-        <v>1825456.65</v>
+        <v>1824260.97</v>
       </c>
       <c r="I50" s="121"/>
       <c r="J50" s="122"/>
@@ -16005,22 +16024,22 @@
       <c r="Q50" s="9"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="308" t="s">
+      <c r="D51" s="298" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="308"/>
+      <c r="E51" s="298"/>
       <c r="F51" s="115">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="309" t="s">
+      <c r="I51" s="299" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="310"/>
-      <c r="K51" s="311">
+      <c r="J51" s="300"/>
+      <c r="K51" s="301">
         <f>F53+F54+F55</f>
-        <v>196737.38</v>
-      </c>
-      <c r="L51" s="312"/>
+        <v>195541.70000000007</v>
+      </c>
+      <c r="L51" s="302"/>
       <c r="P51" s="34"/>
       <c r="Q51" s="9"/>
     </row>
@@ -16044,18 +16063,18 @@
       </c>
       <c r="F53" s="115">
         <f>SUM(F50:F52)</f>
-        <v>-22679.989999999991</v>
+        <v>-23875.669999999925</v>
       </c>
       <c r="H53" s="24"/>
       <c r="I53" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J53" s="130"/>
-      <c r="K53" s="313">
+      <c r="K53" s="303">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="314"/>
+      <c r="L53" s="304"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="131" t="s">
@@ -16072,22 +16091,22 @@
       <c r="C55" s="133">
         <v>44647</v>
       </c>
-      <c r="D55" s="290" t="s">
+      <c r="D55" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="291"/>
+      <c r="E55" s="281"/>
       <c r="F55" s="134">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="292" t="s">
+      <c r="I55" s="282" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="293"/>
-      <c r="K55" s="294">
+      <c r="J55" s="283"/>
+      <c r="K55" s="284">
         <f>K51+K53</f>
-        <v>12395.190000000002</v>
-      </c>
-      <c r="L55" s="294"/>
+        <v>11199.510000000068</v>
+      </c>
+      <c r="L55" s="284"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="135"/>
@@ -16230,19 +16249,10 @@
       <c r="F77" s="150"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
+  <sortState ref="J34:L38">
+    <sortCondition ref="J34:J38"/>
+  </sortState>
+  <mergeCells count="21">
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -16252,7 +16262,18 @@
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="M49:N49"/>
-    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17703,8 +17724,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17727,23 +17748,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="277"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="305"/>
+      <c r="C1" s="307" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="278"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -17753,21 +17774,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="281" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="282"/>
+      <c r="B3" s="309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="310"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="311" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="283"/>
+      <c r="I3" s="311"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="288" t="s">
+      <c r="R3" s="278" t="s">
         <v>38</v>
       </c>
     </row>
@@ -17782,14 +17803,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="284" t="s">
+      <c r="E4" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="H4" s="286" t="s">
+      <c r="F4" s="313"/>
+      <c r="H4" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="287"/>
+      <c r="I4" s="315"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -17799,11 +17820,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="295" t="s">
+      <c r="P4" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="289"/>
+      <c r="Q4" s="286"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -19438,19 +19459,20 @@
       <c r="H40" s="37"/>
       <c r="I40" s="88"/>
       <c r="J40" s="73">
-        <v>44676</v>
-      </c>
-      <c r="K40" s="246" t="s">
-        <v>190</v>
+        <v>44651</v>
+      </c>
+      <c r="K40" s="245" t="s">
+        <v>204</v>
       </c>
       <c r="L40" s="75">
-        <v>30225</v>
-      </c>
-      <c r="M40" s="297">
+        <f>927.48+128</f>
+        <v>1055.48</v>
+      </c>
+      <c r="M40" s="287">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="299">
+      <c r="N40" s="289">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -19474,17 +19496,16 @@
       <c r="H41" s="260"/>
       <c r="I41" s="88"/>
       <c r="J41" s="73">
-        <v>44651</v>
-      </c>
-      <c r="K41" s="245" t="s">
-        <v>204</v>
+        <v>44658</v>
+      </c>
+      <c r="K41" s="76" t="s">
+        <v>323</v>
       </c>
       <c r="L41" s="75">
-        <f>927.48+128</f>
-        <v>1055.48</v>
-      </c>
-      <c r="M41" s="298"/>
-      <c r="N41" s="300"/>
+        <v>1195.68</v>
+      </c>
+      <c r="M41" s="288"/>
+      <c r="N41" s="290"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -19523,13 +19544,13 @@
       <c r="H43" s="37"/>
       <c r="I43" s="95"/>
       <c r="J43" s="73">
-        <v>44681</v>
-      </c>
-      <c r="K43" s="76" t="s">
-        <v>320</v>
+        <v>44676</v>
+      </c>
+      <c r="K43" s="246" t="s">
+        <v>190</v>
       </c>
       <c r="L43" s="80">
-        <v>1498.61</v>
+        <v>30225</v>
       </c>
       <c r="M43" s="96"/>
       <c r="N43" s="97"/>
@@ -19545,10 +19566,18 @@
       <c r="F44" s="245"/>
       <c r="G44" s="261"/>
       <c r="H44" s="37"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="76"/>
-      <c r="L44" s="80"/>
+      <c r="I44" s="95">
+        <v>7</v>
+      </c>
+      <c r="J44" s="73">
+        <v>44681</v>
+      </c>
+      <c r="K44" s="76" t="s">
+        <v>320</v>
+      </c>
+      <c r="L44" s="80">
+        <v>1498.61</v>
+      </c>
       <c r="M44" s="96"/>
       <c r="N44" s="97"/>
       <c r="P44" s="34"/>
@@ -19685,7 +19714,7 @@
       </c>
       <c r="I51" s="111">
         <f>SUM(I5:I50)</f>
-        <v>5682</v>
+        <v>5689</v>
       </c>
       <c r="J51" s="112"/>
       <c r="K51" s="113" t="s">
@@ -19693,7 +19722,7 @@
       </c>
       <c r="L51" s="114">
         <f>SUM(L5:L50)</f>
-        <v>84388.09</v>
+        <v>85583.77</v>
       </c>
       <c r="M51" s="115"/>
       <c r="N51" s="115"/>
@@ -19711,32 +19740,32 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="301" t="s">
+      <c r="H53" s="291" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="302"/>
+      <c r="I53" s="292"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="303">
+      <c r="K53" s="293">
         <f>I51+L51</f>
-        <v>90070.09</v>
-      </c>
-      <c r="L53" s="304"/>
-      <c r="M53" s="305">
+        <v>91272.77</v>
+      </c>
+      <c r="L53" s="294"/>
+      <c r="M53" s="295">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="306"/>
+      <c r="N53" s="296"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="307" t="s">
+      <c r="D54" s="297" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="307"/>
+      <c r="E54" s="297"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>2181081.91</v>
+        <v>2179879.23</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -19744,22 +19773,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="308" t="s">
+      <c r="D55" s="298" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="308"/>
+      <c r="E55" s="298"/>
       <c r="F55" s="115">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="309" t="s">
+      <c r="I55" s="299" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="310"/>
-      <c r="K55" s="311">
+      <c r="J55" s="300"/>
+      <c r="K55" s="301">
         <f>F57+F58+F59</f>
-        <v>262724.02000000019</v>
-      </c>
-      <c r="L55" s="312"/>
+        <v>261521.34000000003</v>
+      </c>
+      <c r="L55" s="302"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -19783,18 +19812,18 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>-46411.569999999832</v>
+        <v>-47614.25</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="313">
+      <c r="K57" s="303">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="314"/>
+      <c r="L57" s="304"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -19811,22 +19840,22 @@
       <c r="C59" s="133">
         <v>44682</v>
       </c>
-      <c r="D59" s="290" t="s">
+      <c r="D59" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="291"/>
+      <c r="E59" s="281"/>
       <c r="F59" s="134">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="292" t="s">
+      <c r="I59" s="282" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="293"/>
-      <c r="K59" s="294">
+      <c r="J59" s="283"/>
+      <c r="K59" s="284">
         <f>K55+K57</f>
-        <v>43306.650000000198</v>
-      </c>
-      <c r="L59" s="294"/>
+        <v>42103.97000000003</v>
+      </c>
+      <c r="L59" s="284"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -19969,19 +19998,10 @@
       <c r="F81" s="150"/>
     </row>
   </sheetData>
+  <sortState ref="J40:L44">
+    <sortCondition ref="J40:J44"/>
+  </sortState>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -19991,6 +20011,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -21445,8 +21477,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="L41" sqref="L41"/>
@@ -21472,23 +21504,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="277"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="305"/>
+      <c r="C1" s="307" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="278"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -21498,21 +21530,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="281" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="282"/>
+      <c r="B3" s="309" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="310"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="311" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="283"/>
+      <c r="I3" s="311"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="288" t="s">
+      <c r="R3" s="278" t="s">
         <v>38</v>
       </c>
     </row>
@@ -21527,14 +21559,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="284" t="s">
+      <c r="E4" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="H4" s="286" t="s">
+      <c r="F4" s="313"/>
+      <c r="H4" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="287"/>
+      <c r="I4" s="315"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -21544,11 +21576,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="295" t="s">
+      <c r="P4" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="289"/>
+      <c r="Q4" s="286"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -23093,17 +23125,17 @@
       <c r="J40" s="73">
         <v>44680</v>
       </c>
-      <c r="K40" s="318" t="s">
+      <c r="K40" s="277" t="s">
         <v>320</v>
       </c>
       <c r="L40" s="75">
         <v>1770.75</v>
       </c>
-      <c r="M40" s="297">
+      <c r="M40" s="287">
         <f>SUM(M5:M39)</f>
         <v>2006096</v>
       </c>
-      <c r="N40" s="299">
+      <c r="N40" s="289">
         <f>SUM(N5:N39)</f>
         <v>61793</v>
       </c>
@@ -23129,8 +23161,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="245"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="298"/>
-      <c r="N41" s="300"/>
+      <c r="M41" s="288"/>
+      <c r="N41" s="290"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -23345,29 +23377,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="301" t="s">
+      <c r="H53" s="291" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="302"/>
+      <c r="I53" s="292"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="303">
+      <c r="K53" s="293">
         <f>I51+L51</f>
         <v>51696.72</v>
       </c>
-      <c r="L53" s="304"/>
-      <c r="M53" s="305">
+      <c r="L53" s="294"/>
+      <c r="M53" s="295">
         <f>N40+M40</f>
         <v>2067889</v>
       </c>
-      <c r="N53" s="306"/>
+      <c r="N53" s="296"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="307" t="s">
+      <c r="D54" s="297" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="307"/>
+      <c r="E54" s="297"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>2048800.2799999998</v>
@@ -23378,22 +23410,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="308" t="s">
+      <c r="D55" s="298" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="308"/>
+      <c r="E55" s="298"/>
       <c r="F55" s="115">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="309" t="s">
+      <c r="I55" s="299" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="310"/>
-      <c r="K55" s="311">
+      <c r="J55" s="300"/>
+      <c r="K55" s="301">
         <f>F57+F58+F59</f>
         <v>-53185.560000000114</v>
       </c>
-      <c r="L55" s="312"/>
+      <c r="L55" s="302"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -23424,11 +23456,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="313">
+      <c r="K57" s="303">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="314"/>
+      <c r="L57" s="304"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -23445,20 +23477,20 @@
       <c r="C59" s="133">
         <v>44710</v>
       </c>
-      <c r="D59" s="290" t="s">
+      <c r="D59" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="291"/>
+      <c r="E59" s="281"/>
       <c r="F59" s="134">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="292"/>
-      <c r="J59" s="293"/>
-      <c r="K59" s="294">
+      <c r="I59" s="282"/>
+      <c r="J59" s="283"/>
+      <c r="K59" s="284">
         <f>K55+K57</f>
         <v>-351060.15000000014</v>
       </c>
-      <c r="L59" s="294"/>
+      <c r="L59" s="284"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -23602,6 +23634,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -23611,18 +23655,6 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>